<commit_message>
Afdi Fauzul Bahar 14117149
</commit_message>
<xml_diff>
--- a/tugas/laporan.xlsx
+++ b/tugas/laporan.xlsx
@@ -1,38 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karunia/Documents/lecturer - DBMS/2019:2020/IF3144-1920/tugas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\PABW\IF3144-1920\tugas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F409652C-A4B2-B041-93C9-55CCCBF85C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{3C9D5799-7662-CB47-8B99-82C16436D226}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Tugas" sheetId="1" r:id="rId1"/>
     <sheet name="Laporan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>advisor = 100, student = 100, section = 200,takes = 200</t>
   </si>
@@ -73,18 +66,6 @@
     <t>SELECT * FROM student WHERE tot_cred &gt; 30;</t>
   </si>
   <si>
-    <t>SELECT * FROM student</t>
-  </si>
-  <si>
-    <t>SELECT `name`, department FROM student WHERE tot_cred &gt; 30;</t>
-  </si>
-  <si>
-    <t>SELECT *  FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id</t>
-  </si>
-  <si>
-    <t>SELECT student.`name`,student.dept_name,takes.sec_id AS pengambilan,takes.semester,section.room_number,section.building,course.course_id,course.dept_name FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id JOIN course ON section.course_id = course.course_id</t>
-  </si>
-  <si>
     <t>1. Run dengan menggunakan terminal Query di atas dan catat waktunya</t>
   </si>
   <si>
@@ -134,12 +115,126 @@
   </si>
   <si>
     <t>4. Lakukan pada setiap Query</t>
+  </si>
+  <si>
+    <t>Query 1</t>
+  </si>
+  <si>
+    <t>Query 2</t>
+  </si>
+  <si>
+    <t>Query 3</t>
+  </si>
+  <si>
+    <t>Query 4</t>
+  </si>
+  <si>
+    <t>Query 5</t>
+  </si>
+  <si>
+    <t>0.00077130</t>
+  </si>
+  <si>
+    <t>0.00081460</t>
+  </si>
+  <si>
+    <t>0.00067920</t>
+  </si>
+  <si>
+    <t>0.19959490</t>
+  </si>
+  <si>
+    <t>0.06971610</t>
+  </si>
+  <si>
+    <t>SELECT `name`, dept_name FROM student WHERE tot_cred &gt; 30;</t>
+  </si>
+  <si>
+    <t>SELECT *  FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id;</t>
+  </si>
+  <si>
+    <t>0.00044380</t>
+  </si>
+  <si>
+    <t>0.00041460</t>
+  </si>
+  <si>
+    <t>0.00038590</t>
+  </si>
+  <si>
+    <t>0.00184840</t>
+  </si>
+  <si>
+    <t>0.00237200</t>
+  </si>
+  <si>
+    <t>0.00052060</t>
+  </si>
+  <si>
+    <t>0.00048710</t>
+  </si>
+  <si>
+    <t>0.00044780</t>
+  </si>
+  <si>
+    <t>0.00352350</t>
+  </si>
+  <si>
+    <t>SELECT * FROM student;</t>
+  </si>
+  <si>
+    <t>SELECT student.`name`,student.dept_name,takes.sec_id AS pengambilan,takes.semester,section.room_number,section.building,course.course_id,course.dept_name FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id JOIN course ON section.course_id = course.course_id;</t>
+  </si>
+  <si>
+    <t>0.00013030</t>
+  </si>
+  <si>
+    <t>0.00010340</t>
+  </si>
+  <si>
+    <t>0.00011860</t>
+  </si>
+  <si>
+    <t>0.00014400</t>
+  </si>
+  <si>
+    <t>0.00023570</t>
+  </si>
+  <si>
+    <t>0.00011050</t>
+  </si>
+  <si>
+    <t>0.00012370</t>
+  </si>
+  <si>
+    <t>0.00010310</t>
+  </si>
+  <si>
+    <t>0.00017800</t>
+  </si>
+  <si>
+    <t>0.00016900</t>
+  </si>
+  <si>
+    <t>0.00014000</t>
+  </si>
+  <si>
+    <t>0.00011270</t>
+  </si>
+  <si>
+    <t>0.00014600</t>
+  </si>
+  <si>
+    <t>0.00045960</t>
+  </si>
+  <si>
+    <t>0.00030480</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -165,7 +260,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -188,16 +283,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,223 +689,386 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7283ED88-C5BB-2349-93B1-5D98200E2DE2}">
-  <dimension ref="A2:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A3" sqref="A3:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.375" hidden="1" customWidth="1"/>
+    <col min="7" max="11" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEE10EE-7B32-C94F-84A3-EE8D948576BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>